<commit_message>
refactor, reset HEAD --soft, update  gitignore
</commit_message>
<xml_diff>
--- a/Code/TopicNumber/Topic_Modeling_Bigram/Evaluation/Coherence_vs_Difference_Hellinger_avg.xlsx
+++ b/Code/TopicNumber/Topic_Modeling_Bigram/Evaluation/Coherence_vs_Difference_Hellinger_avg.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataScience\Code\TopicNumber\Topic_Modeling_Bigram\Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DataScience\BachelorTopicModeling\Code\TopicNumber\Topic_Modeling_Bigram\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A6CC14-4BD2-4532-8F8D-9E377F9D2709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D714419D-375E-4D94-9DF0-D877EC9AA5C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1650" windowWidth="21900" windowHeight="14295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coherence_vs_Difference" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Kohärenz: u_mass</t>
+  </si>
+  <si>
+    <t>Distanz: Hellinger Mittelwert</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2546,6 +2557,1018 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coherence_vs_Difference!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kohärenz: u_mass</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Coherence_vs_Difference!$B$2:$CW$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0.28584917297358498</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.74604827280641</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4564694275752998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7063206594575</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2696210570534201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6762909642435599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.80244558370492</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.80981322662022</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0737077576146898</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.13371694918655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7564888894561701</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4687320816237599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2832040762698198</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.8572032819356599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.73039968780459</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.8897349050769301</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9277744288012899</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.8355836265674799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0642961696420099</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.2837070741172001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.18407077960588</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.8134675867346099</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4226825920647799</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.5190743152187798</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.2540952904893201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.2805007167840201</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.2777072696935301</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.5929476994060798</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1499568414489101</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.2158144246049698</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.1886297931572098</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.3580931758064496</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.8175079816773003</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0442203822908898</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.6808036576216603</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4465868940108901</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.5268407780558304</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.4819966044197201</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.6741589114155504</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.7712105987183397</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.8392309804161702</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.1325716854654502</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.3250952097195503</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.4247868363565299</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.5390834367503201</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.6402130088406901</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.7280193625926001</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.8975517117406602</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.89720560013855</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.8144342032063596</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6.1562049531906498</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.0044575303431804</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.9308262109811496</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.0206291735575999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.8923470929403399</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.1054149098655399</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.0529596194266002</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.9540013689017197</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.7903898294948997</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.77365325408031</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.6016118891675504</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.8983681221923803</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.9305286538063902</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.9017299732001396</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.9520356224455204</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.1314889268381503</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.0573170890513</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.1213035054928904</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.1013444418230103</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.2753440395373401</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>6.1773256003077499</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>6.09434677932156</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.80824150482864</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.9157335536969002</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.8629561190194197</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.9553693859263896</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5.8542871549475599</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.0996597357425699</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.0864289416346802</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.17434296183146</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.1159453401998798</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.9788765592810096</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.1519423829286</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.0970574321889002</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>6.07326212722002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6.1579105280536099</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.1309253164147997</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.1911822790444297</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.27632386940759</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.39917033273586</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.4431180329957796</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.5149947148026399</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.3296375270344001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.3781289206457901</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.3730897232133401</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.3085686779058703</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.3481551020543296</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.3283696987081797</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.5333181251132801</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.5449348947718304</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DAA-4DED-A540-E4430C4D48B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1376952367"/>
+        <c:axId val="1174296351"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Coherence_vs_Difference!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Distanz: Hellinger Mittelwert</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Coherence_vs_Difference!$B$3:$CW$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89878801778579698</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87718500843860003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86599694642112401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85720825933691802</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.85932070394228999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86649731737264801</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.86267862497388303</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.864265658782433</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.86798013650694605</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.85993168313130497</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86093414987031303</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.86553957621025701</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.85764394876728101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.854929574276453</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.85733104504955004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.86107714107829003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.86492320609268503</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.87098737718172203</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.870020992311902</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.87035454567988702</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.870357780916588</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.87082363084915604</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.87176205302615695</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.87490758172402805</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.87683457845558599</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.87828093083348802</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87859478253707302</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.87877451018392105</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.87970134616117701</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.88054004665310204</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.87197754052675702</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.87116262571220104</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.88391621597858305</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.88077063279994094</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.87840609755177901</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.88039638560173905</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.88012745960199901</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.88069356299522505</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.88422247114683294</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.88571215389268498</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.88885940077432601</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.88935778921698905</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.88063480707480302</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.88146748658740504</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.88197402719200302</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.88206362823425299</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.88288937716486104</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.88284578587290796</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.88281012948135995</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.88503669630855597</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.88800879296296098</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.88868026177870196</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.88902853613580901</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.893471874802792</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.89424333425346103</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89371415873441695</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.89199913482886795</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.892217139588522</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.89413274525639896</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.89328916899587896</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.89364559230714602</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.89348921317969399</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.89414967718438498</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.89556357646098295</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.89520759075830603</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.89559044439245095</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.89500361870253198</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89603245717880098</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.89584236153350305</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.895341586317972</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.89630546524531796</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.89734576908376495</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.89710161970727698</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.89778448510435704</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.89716506594136602</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.89265310448318202</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.89299498281449496</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.89334293492229</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.894895298043763</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.89458022609145804</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.89499640715540496</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.89501303144839905</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.89560860876714898</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.89482586741529302</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.89666155677050097</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.89626418313655698</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.89626654182425702</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89758859907865596</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.89798221266122702</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.898491252235743</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.89860700254105097</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.89821579561283504</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.89816056439748504</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.898616550408047</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.89958126637980895</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.901161195281029</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.90123073043020596</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.90092862658194295</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9DAA-4DED-A540-E4430C4D48B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1377477711"/>
+        <c:axId val="1174295935"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1376952367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1174296351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1174296351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1376952367"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1174295935"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.9"/>
+          <c:min val="0.85000000000000009"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1377477711"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1377477711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1174295935"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2666,6 +3689,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -3861,6 +4924,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4319,6 +5885,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6629C7FD-D601-42CB-9A81-77D04F70797F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4626,8 +6228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4935,7 +6537,7 @@
       </c>
     </row>
     <row r="2" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -5240,7 +6842,7 @@
       </c>
     </row>
     <row r="3" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">

</xml_diff>